<commit_message>
adding test cases and common data providers
</commit_message>
<xml_diff>
--- a/src/test/resources/com/w2a/excel/testdata.xlsx
+++ b/src/test/resources/com/w2a/excel/testdata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\IntelliJ\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\IntelliJ\Udemy\Architect\PageObjectModelBasics\src\test\resources\com\w2a\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255F61E4-7D57-4169-8A11-580CEA59C259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905037CF-FD40-4FA5-A464-6C67740F7CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId2"/>
+    <sheet name="createAccountTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,88 +35,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Raman</t>
   </si>
   <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>A234wd</t>
-  </si>
-  <si>
-    <t>alert</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Raman Arora</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Ishita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Sehgal</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
-    <t>BankManangerLoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
     <t>Runmode</t>
   </si>
   <si>
     <t>runmode</t>
   </si>
   <si>
-    <t>N</t>
+    <t>LoginTest</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>test.automatisierer@gmail.com</t>
+  </si>
+  <si>
+    <t>Selenium@123</t>
+  </si>
+  <si>
+    <t>CreateAccountTest</t>
+  </si>
+  <si>
+    <t>accountname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,13 +111,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -486,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDB6888-7696-4AF5-B1FE-58A9156BB586}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,34 +474,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -537,134 +504,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1DC5759E-7B06-42E6-9AE6-9728F815A879}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{4BE6A518-4E6E-43F7-A281-2BA42961CD18}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D709006C-3DF3-4AF9-A7D7-336DD711B299}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC343F5-901A-45D0-B097-EE83E29D70AB}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>